<commit_message>
Done service discovery And Gateway
</commit_message>
<xml_diff>
--- a/exports/output_user_data.xlsx
+++ b/exports/output_user_data.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Danh sách User</t>
   </si>
@@ -116,37 +116,34 @@
     <t>id</t>
   </si>
   <si>
+    <t>tejst5</t>
+  </si>
+  <si>
+    <t>test5j@gmail.com</t>
+  </si>
+  <si>
+    <t>Đạt</t>
+  </si>
+  <si>
+    <t>Phan</t>
+  </si>
+  <si>
+    <t>Đường Ok</t>
+  </si>
+  <si>
+    <t>Tam Thuấn</t>
+  </si>
+  <si>
+    <t>Phúc Thọ</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
     <t>dat2k3</t>
   </si>
   <si>
     <t>dat2k3@gmail.com</t>
-  </si>
-  <si>
-    <t>Đạt</t>
-  </si>
-  <si>
-    <t>Phan</t>
-  </si>
-  <si>
-    <t>Đường Ok</t>
-  </si>
-  <si>
-    <t>Tam Thuấn</t>
-  </si>
-  <si>
-    <t>Phúc Thọ</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>bossday</t>
-  </si>
-  <si>
-    <t>ytbs1vn@gmail.com</t>
-  </si>
-  <si>
-    <t>Dat Do Doc</t>
   </si>
 </sst>
 </file>
@@ -667,7 +664,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2" ht="18.0" customHeight="true">
       <c r="A3" s="4" t="n">
-        <v>2.0</v>
+        <v>52.0</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>23</v>
@@ -702,7 +699,7 @@
     </row>
     <row r="4" ht="18.0" customHeight="true">
       <c r="A4" t="n" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B4" t="s" s="5">
         <v>31</v>
@@ -711,18 +708,28 @@
         <v>32</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="F4" t="n" s="7">
+        <v>36572.0</v>
+      </c>
+      <c r="G4" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s" s="3">
+        <v>30</v>
+      </c>
       <c r="K4" t="n" s="6">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>